<commit_message>
bolts: FlatWasher class created, documented and tested
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/VER1_ReferenceFlange-Results.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/VER1_ReferenceFlange-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B065BCA3-62C0-4BB5-833C-0A73CA293D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11BA4F3-DC51-4F15-A196-2F5C48A121CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="28680" yWindow="-11130" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5174,6 +5174,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5201,17 +5210,8 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -19763,32 +19763,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -19804,12 +19804,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19817,12 +19817,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19830,12 +19830,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19843,12 +19843,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19856,12 +19856,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19909,112 +19909,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="174" t="s">
+      <c r="C17" s="164"/>
+      <c r="D17" s="162" t="s">
         <v>327</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20202,16 +20202,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24164,16 +24164,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24184,6 +24174,16 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24269,32 +24269,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -24310,12 +24310,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24323,12 +24323,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24336,12 +24336,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24349,12 +24349,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24362,12 +24362,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24415,117 +24415,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24713,16 +24713,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28648,13 +28648,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28668,6 +28661,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -28753,32 +28753,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -28794,12 +28794,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28807,12 +28807,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28820,12 +28820,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28833,12 +28833,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28846,12 +28846,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28899,117 +28899,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29197,16 +29197,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33132,13 +33132,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33152,6 +33145,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33237,32 +33237,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -33278,12 +33278,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33291,12 +33291,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33304,12 +33304,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33317,12 +33317,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33330,12 +33330,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33383,117 +33383,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33681,16 +33681,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37616,13 +37616,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37636,6 +37629,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -37670,10 +37670,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE0C33B-3A47-45F1-AB71-67A51F114D32}">
   <sheetPr codeName="Tabelle12"/>
-  <dimension ref="A1:X120"/>
+  <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -38485,7 +38485,7 @@
       </c>
       <c r="E38" s="109" cm="1">
         <f t="array" ref="E38">INDEX(N38:Q38,case_number)</f>
-        <v>0.1284830227486351</v>
+        <v>0.14347872373893336</v>
       </c>
       <c r="F38" s="109" cm="1">
         <f t="array" aca="1" ref="F38" ca="1">INDIRECT(sheet_name&amp;"!bolt.axial_stiffness")/(INDIRECT(sheet_name&amp;"!bolt.axial_stiffness")+INDIRECT(sheet_name&amp;"!clamped_parts_stiffness"))</f>
@@ -38493,7 +38493,7 @@
       </c>
       <c r="G38" s="118">
         <f ca="1">(F38-E38)/E38</f>
-        <v>9.8899776334887037E-4</v>
+        <v>-0.10362952206924958</v>
       </c>
       <c r="H38" s="150"/>
       <c r="I38" s="143"/>
@@ -38506,16 +38506,16 @@
         <v>123</v>
       </c>
       <c r="N38" s="109">
-        <v>0.1284830227486351</v>
+        <v>0.14347872373893336</v>
       </c>
       <c r="O38" s="109">
-        <v>0.1284830227486351</v>
+        <v>0.14347872373893336</v>
       </c>
       <c r="P38" s="109">
-        <v>0.1284830227486351</v>
+        <v>0.14347872373893336</v>
       </c>
       <c r="Q38" s="109">
-        <v>0.1284830227486351</v>
+        <v>0.14347872373893336</v>
       </c>
       <c r="R38" t="str">
         <f t="shared" si="1"/>
@@ -39976,7 +39976,7 @@
       </c>
       <c r="E72" s="107" cm="1">
         <f t="array" ref="E72">INDEX(N72:Q72,case_number)</f>
-        <v>819.26437142240161</v>
+        <v>820.46246254221171</v>
       </c>
       <c r="F72" s="107" cm="1">
         <f t="array" aca="1" ref="F72" ca="1">INDIRECT(sheet_name&amp;"!Point3.Fs")</f>
@@ -39984,7 +39984,7 @@
       </c>
       <c r="G72" s="118">
         <f t="shared" ca="1" si="5"/>
-        <v>6.0267065949214003E-5</v>
+        <v>-1.4000841139623081E-3</v>
       </c>
       <c r="K72" s="106"/>
       <c r="L72" s="103" t="s">
@@ -39994,16 +39994,16 @@
         <v>128</v>
       </c>
       <c r="N72" s="109">
-        <v>819.26437142240161</v>
+        <v>820.46246254221171</v>
       </c>
       <c r="O72" s="109">
-        <v>813.00847802715259</v>
+        <v>813.47642204444719</v>
       </c>
       <c r="P72" s="109">
-        <v>812.11238963316589</v>
+        <v>812.4757480536274</v>
       </c>
       <c r="Q72" s="109">
-        <v>811.76736347545329</v>
+        <v>812.09045269159333</v>
       </c>
     </row>
     <row r="73" spans="2:18" ht="15.6">
@@ -40046,7 +40046,7 @@
       <c r="D74" s="103"/>
       <c r="E74" s="107" cm="1">
         <f t="array" ref="E74">INDEX(N74:Q74,case_number)</f>
-        <v>19777.636510175686</v>
+        <v>19064.61660154846</v>
       </c>
       <c r="F74" s="111" t="s">
         <v>86</v>
@@ -40058,16 +40058,16 @@
       </c>
       <c r="M74" s="103"/>
       <c r="N74" s="111">
-        <v>19777.636510175686</v>
+        <v>19064.61660154846</v>
       </c>
       <c r="O74" s="111">
-        <v>18124.980347259152</v>
+        <v>17829.687383462817</v>
       </c>
       <c r="P74" s="111">
-        <v>18038.43652663703</v>
+        <v>17807.163701545032</v>
       </c>
       <c r="Q74" s="111">
-        <v>18015.548639630913</v>
+        <v>17809.23919208629</v>
       </c>
     </row>
     <row r="75" spans="2:18" ht="15.6">
@@ -40078,7 +40078,7 @@
       <c r="D75" s="103"/>
       <c r="E75" s="107" cm="1">
         <f t="array" ref="E75">INDEX(N75:Q75,case_number)</f>
-        <v>2549337.1154325213</v>
+        <v>2930697.3626370565</v>
       </c>
       <c r="F75" s="111" t="s">
         <v>86</v>
@@ -40090,16 +40090,16 @@
       </c>
       <c r="M75" s="103"/>
       <c r="N75" s="111">
-        <v>2549337.1154325213</v>
+        <v>2930697.3626370565</v>
       </c>
       <c r="O75" s="111">
-        <v>1238490.9765994144</v>
+        <v>1407034.0362689719</v>
       </c>
       <c r="P75" s="111">
-        <v>985749.82509730884</v>
+        <v>1119011.3051081342</v>
       </c>
       <c r="Q75" s="111">
-        <v>883930.78411035344</v>
+        <v>1003234.3358982865</v>
       </c>
     </row>
     <row r="76" spans="2:18" ht="15.6">
@@ -40110,7 +40110,7 @@
       <c r="D76" s="103"/>
       <c r="E76" s="148" cm="1">
         <f t="array" ref="E76">INDEX(N76:Q76,case_number)</f>
-        <v>7.4452549368613549E-4</v>
+        <v>7.1768399019275309E-4</v>
       </c>
       <c r="F76" s="148" cm="1">
         <f t="array" aca="1" ref="F76" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.2")*1000</f>
@@ -40118,7 +40118,7 @@
       </c>
       <c r="G76" s="118">
         <f t="shared" ref="G76:G78" ca="1" si="6">(F76-E76)/E76</f>
-        <v>-1.2940860171702375E-2</v>
+        <v>2.3975319807121687E-2</v>
       </c>
       <c r="K76" s="106"/>
       <c r="L76" s="105" t="s">
@@ -40126,16 +40126,16 @@
       </c>
       <c r="M76" s="103"/>
       <c r="N76" s="139">
-        <v>7.4452549368613549E-4</v>
+        <v>7.1768399019275309E-4</v>
       </c>
       <c r="O76" s="139">
-        <v>7.2924237999581396E-4</v>
+        <v>7.1736153159823648E-4</v>
       </c>
       <c r="P76" s="139">
-        <v>7.324493438548949E-4</v>
+        <v>7.2305852837374401E-4</v>
       </c>
       <c r="Q76" s="139">
-        <v>7.3417218017621602E-4</v>
+        <v>7.2576462845938463E-4</v>
       </c>
     </row>
     <row r="77" spans="2:18" ht="15.6">
@@ -40146,7 +40146,7 @@
       <c r="D77" s="103"/>
       <c r="E77" s="148" cm="1">
         <f t="array" ref="E77">INDEX(N77:Q77,case_number)</f>
-        <v>9.5969327450387346E-2</v>
+        <v>0.1103255639084767</v>
       </c>
       <c r="F77" s="148" cm="1">
         <f t="array" aca="1" ref="F77" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.1")</f>
@@ -40154,7 +40154,7 @@
       </c>
       <c r="G77" s="118">
         <f t="shared" ca="1" si="6"/>
-        <v>1.471206963892776E-3</v>
+        <v>-0.12884634541289705</v>
       </c>
       <c r="K77" s="106"/>
       <c r="L77" s="105" t="s">
@@ -40162,16 +40162,16 @@
       </c>
       <c r="M77" s="103"/>
       <c r="N77" s="139">
-        <v>9.5969327450387346E-2</v>
+        <v>0.1103255639084767</v>
       </c>
       <c r="O77" s="139">
-        <v>4.982957719539112E-2</v>
+        <v>5.6610756518644334E-2</v>
       </c>
       <c r="P77" s="139">
-        <v>4.0026296709885008E-2</v>
+        <v>4.5437368974985494E-2</v>
       </c>
       <c r="Q77" s="139">
-        <v>3.6022072037683199E-2</v>
+        <v>4.0883947214009071E-2</v>
       </c>
     </row>
     <row r="78" spans="2:18" ht="14.4">
@@ -40182,7 +40182,7 @@
       <c r="D78" s="103"/>
       <c r="E78" s="108" cm="1">
         <f t="array" ref="E78">INDEX(N78:Q78,case_number)</f>
-        <v>811.21525537115815</v>
+        <v>811.67231793674671</v>
       </c>
       <c r="F78" s="107" cm="1">
         <f t="array" aca="1" ref="F78" ca="1">INDIRECT(sheet_name&amp;"!Fs_coeff.tens.0")/1000</f>
@@ -40190,7 +40190,7 @@
       </c>
       <c r="G78" s="118">
         <f t="shared" ca="1" si="6"/>
-        <v>1.7103629807629394E-5</v>
+        <v>-5.4601817799202737E-4</v>
       </c>
       <c r="K78" s="106"/>
       <c r="L78" s="112" t="s">
@@ -40198,16 +40198,16 @@
       </c>
       <c r="M78" s="103"/>
       <c r="N78" s="108">
-        <v>811.21525537115815</v>
+        <v>811.67231793674671</v>
       </c>
       <c r="O78" s="108">
-        <v>809.83853702127681</v>
+        <v>810.05370623124679</v>
       </c>
       <c r="P78" s="108">
-        <v>809.54016398594285</v>
+        <v>809.71177786358919</v>
       </c>
       <c r="Q78" s="108">
-        <v>809.41791616056889</v>
+        <v>809.57208469795864</v>
       </c>
     </row>
     <row r="79" spans="2:18" ht="15.6">
@@ -41559,7 +41559,7 @@
       </c>
       <c r="E107" s="113" cm="1">
         <f t="array" ref="E107">INDEX(N107:Q107,case_number)</f>
-        <v>5.1165437741928325E-2</v>
+        <v>6.7136936231689967E-2</v>
       </c>
       <c r="F107" s="113" cm="1">
         <f t="array" aca="1" ref="F107" ca="1">INDIRECT(sheet_name&amp;"!true_force_initial_slope")</f>
@@ -41567,7 +41567,7 @@
       </c>
       <c r="G107" s="118">
         <f ca="1">(F107-E107)/E107</f>
-        <v>1.2651885031172655E-2</v>
+        <v>-0.22825228725060343</v>
       </c>
       <c r="I107" s="105"/>
       <c r="K107" s="106">
@@ -41581,16 +41581,16 @@
         <v>123</v>
       </c>
       <c r="N107" s="109">
-        <v>5.1165437741928325E-2</v>
+        <v>6.7136936231689967E-2</v>
       </c>
       <c r="O107" s="109">
-        <v>5.9453913058859212E-3</v>
+        <v>1.3441533684499327E-2</v>
       </c>
       <c r="P107" s="109">
-        <v>-4.0508771371605117E-3</v>
+        <v>1.9253135360486067E-3</v>
       </c>
       <c r="Q107" s="109">
-        <v>-8.1587782699442616E-3</v>
+        <v>-2.7909553159588146E-3</v>
       </c>
       <c r="R107" t="str">
         <f t="shared" si="7"/>
@@ -41610,7 +41610,7 @@
       </c>
       <c r="E108" s="108" cm="1">
         <f t="array" ref="E108">INDEX(N108:Q108,case_number)</f>
-        <v>799.60607889636435</v>
+        <v>796.67399742767748</v>
       </c>
       <c r="F108" s="108" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">INDIRECT(sheet_name&amp;"!point4.Fs")</f>
@@ -41618,7 +41618,7 @@
       </c>
       <c r="G108" s="118">
         <f ca="1">(F108-E108)/E108</f>
-        <v>-1.47550166126383E-4</v>
+        <v>3.5323099134605754E-3</v>
       </c>
       <c r="I108" s="103"/>
       <c r="K108" s="106">
@@ -41632,16 +41632,16 @@
         <v>128</v>
       </c>
       <c r="N108" s="108">
-        <v>799.60607889636435</v>
+        <v>796.67399742767748</v>
       </c>
       <c r="O108" s="108">
-        <v>808.46486080688624</v>
+        <v>807.79122657473408</v>
       </c>
       <c r="P108" s="108">
-        <v>809.29077292038016</v>
+        <v>808.86052908007298</v>
       </c>
       <c r="Q108" s="108">
-        <v>809.52766803795828</v>
+        <v>809.17993768937845</v>
       </c>
       <c r="R108" t="str">
         <f t="shared" si="7"/>
@@ -41661,7 +41661,7 @@
       </c>
       <c r="E109" s="110" cm="1">
         <f t="array" ref="E109">INDEX(N109:Q109,case_number)</f>
-        <v>0.11662403043349931</v>
+        <v>0.13023562713515596</v>
       </c>
       <c r="F109" s="104"/>
       <c r="G109" s="104"/>
@@ -41680,16 +41680,16 @@
         <v>123</v>
       </c>
       <c r="N109" s="113">
-        <v>0.11662403043349931</v>
+        <v>0.13023562713515596</v>
       </c>
       <c r="O109" s="113">
-        <v>5.7087891074944296E-2</v>
+        <v>6.375081763452102E-2</v>
       </c>
       <c r="P109" s="113">
-        <v>4.5734916845549152E-2</v>
+        <v>5.1072798249334042E-2</v>
       </c>
       <c r="Q109" s="113">
-        <v>4.1153055945649206E-2</v>
+        <v>4.5956172408789291E-2</v>
       </c>
       <c r="R109" t="str">
         <f t="shared" si="7"/>
@@ -41709,7 +41709,7 @@
       </c>
       <c r="E110" s="110" cm="1">
         <f t="array" ref="E110">INDEX(N110:Q110,case_number)</f>
-        <v>0.11662403043349931</v>
+        <v>0.13023562713515596</v>
       </c>
       <c r="F110" s="104"/>
       <c r="G110" s="104"/>
@@ -41728,16 +41728,16 @@
         <v>123</v>
       </c>
       <c r="N110" s="113">
-        <v>0.11662403043349931</v>
+        <v>0.13023562713515596</v>
       </c>
       <c r="O110" s="113">
-        <v>5.7087891074944296E-2</v>
+        <v>6.375081763452102E-2</v>
       </c>
       <c r="P110" s="113">
-        <v>4.5734916845549152E-2</v>
+        <v>5.1072798249334042E-2</v>
       </c>
       <c r="Q110" s="113">
-        <v>4.1153055945649206E-2</v>
+        <v>4.5956172408789291E-2</v>
       </c>
       <c r="R110" t="str">
         <f t="shared" si="7"/>
@@ -42004,7 +42004,7 @@
       </c>
       <c r="E117" s="113" cm="1">
         <f t="array" ref="E117">INDEX(N117:Q117,case_number)</f>
-        <v>0.19967104328349522</v>
+        <v>0.22881533152730013</v>
       </c>
       <c r="F117" s="113" cm="1">
         <f t="array" aca="1" ref="F117" ca="1">INDIRECT(sheet_name&amp;"!true_moment_initial_slope")</f>
@@ -42012,7 +42012,7 @@
       </c>
       <c r="G117" s="118">
         <f ca="1">(F117-E117)/E117</f>
-        <v>-1.33464683443769E-2</v>
+        <v>-0.13901687133443508</v>
       </c>
       <c r="H117" t="s">
         <v>309</v>
@@ -42029,16 +42029,16 @@
         <v>123</v>
       </c>
       <c r="N117" s="109">
-        <v>0.19967104328349522</v>
+        <v>0.22881533152730013</v>
       </c>
       <c r="O117" s="109">
-        <v>0.16432289632462671</v>
+        <v>0.17800162123193988</v>
       </c>
       <c r="P117" s="109">
-        <v>0.1548186279410291</v>
+        <v>0.16572379276896795</v>
       </c>
       <c r="Q117" s="109">
-        <v>0.15084002522695492</v>
+        <v>0.16063505977007558</v>
       </c>
       <c r="R117" t="str">
         <f t="shared" si="7"/>
@@ -42054,7 +42054,7 @@
       </c>
       <c r="E118" s="113" cm="1">
         <f t="array" ref="E118">INDEX(N118:Q118,case_number)</f>
-        <v>0.54369949524356476</v>
+        <v>0.15821187587621519</v>
       </c>
       <c r="F118" s="109" t="s">
         <v>86</v>
@@ -42072,16 +42072,16 @@
         <v>123</v>
       </c>
       <c r="N118" s="114">
-        <v>0.54369949524356476</v>
+        <v>0.15821187587621519</v>
       </c>
       <c r="O118" s="114">
-        <v>0.55006886815760159</v>
+        <v>8.2396184802145889E-2</v>
       </c>
       <c r="P118" s="114">
-        <v>0.54902760124831862</v>
+        <v>6.1809102945987966E-2</v>
       </c>
       <c r="Q118" s="114">
-        <v>0.54838075370525208</v>
+        <v>5.2825300178790752E-2</v>
       </c>
       <c r="R118" t="str">
         <f t="shared" si="7"/>
@@ -42101,7 +42101,7 @@
       </c>
       <c r="E119" s="108" cm="1">
         <f t="array" ref="E119">INDEX(N119:Q119,case_number)</f>
-        <v>-39.859975939219623</v>
+        <v>-45.210346008284084</v>
       </c>
       <c r="F119" s="108" cm="1">
         <f t="array" aca="1" ref="F119" ca="1">INDIRECT(sheet_name&amp;"!point4.Ms")</f>
@@ -42109,7 +42109,7 @@
       </c>
       <c r="G119" s="118">
         <f ca="1">(F119-E119)/E119</f>
-        <v>-1.4625023383427124E-2</v>
+        <v>-0.13123817163777518</v>
       </c>
       <c r="H119" t="s">
         <v>309</v>
@@ -42126,16 +42126,16 @@
         <v>121</v>
       </c>
       <c r="N119" s="108">
-        <v>-39.859975939219623</v>
+        <v>-45.210346008284084</v>
       </c>
       <c r="O119" s="108">
-        <v>-19.392266160885868</v>
+        <v>-20.621492726278412</v>
       </c>
       <c r="P119" s="108">
-        <v>-16.034701537802789</v>
+        <v>-16.819796969210302</v>
       </c>
       <c r="Q119" s="108">
-        <v>-14.76634987060744</v>
+        <v>-15.400877276825481</v>
       </c>
       <c r="R119" t="str">
         <f t="shared" si="7"/>
@@ -42151,7 +42151,7 @@
       </c>
       <c r="E120" s="108" cm="1">
         <f t="array" ref="E120">INDEX(N120:Q120,case_number)</f>
-        <v>-397.15543922091894</v>
+        <v>-33.319505980114876</v>
       </c>
       <c r="F120" s="109" t="s">
         <v>86</v>
@@ -42169,20 +42169,222 @@
         <v>121</v>
       </c>
       <c r="N120" s="108">
-        <v>-397.15543922091894</v>
+        <v>-33.319505980114876</v>
       </c>
       <c r="O120" s="108">
-        <v>-404.48917844359784</v>
+        <v>-10.142393084455744</v>
       </c>
       <c r="P120" s="108">
-        <v>-408.28964979396551</v>
+        <v>-6.7655530926182665</v>
       </c>
       <c r="Q120" s="108">
-        <v>-410.13082561232886</v>
+        <v>-5.5527024742467699</v>
       </c>
       <c r="R120" t="str">
         <f t="shared" si="7"/>
         <v>(valid in case T-Flange is calculated)</v>
+      </c>
+    </row>
+    <row r="121" spans="2:18">
+      <c r="N121" s="109">
+        <v>-30.038888888888888</v>
+      </c>
+      <c r="O121" s="109">
+        <v>-30.038888888888888</v>
+      </c>
+      <c r="P121" s="109">
+        <v>-30.038888888888888</v>
+      </c>
+      <c r="Q121" s="109">
+        <v>-30.038888888888888</v>
+      </c>
+    </row>
+    <row r="122" spans="2:18">
+      <c r="N122" s="113">
+        <v>0</v>
+      </c>
+      <c r="O122" s="113">
+        <v>0</v>
+      </c>
+      <c r="P122" s="113">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:18">
+      <c r="N123" s="109">
+        <v>-12.975440564878406</v>
+      </c>
+      <c r="O123" s="109">
+        <v>-14.122778963275536</v>
+      </c>
+      <c r="P123" s="109">
+        <v>-14.335292780869318</v>
+      </c>
+      <c r="Q123" s="109">
+        <v>-14.420851032204688</v>
+      </c>
+    </row>
+    <row r="124" spans="2:18">
+      <c r="N124" s="113">
+        <v>-4.2746352261146034</v>
+      </c>
+      <c r="O124" s="113">
+        <v>-2.7379325128683178</v>
+      </c>
+      <c r="P124" s="113">
+        <v>-2.3157309113001991</v>
+      </c>
+      <c r="Q124" s="113">
+        <v>-2.1306521938137162</v>
+      </c>
+    </row>
+    <row r="125" spans="2:18">
+      <c r="N125" s="113">
+        <v>4.1738389339481133E-3</v>
+      </c>
+      <c r="O125" s="113">
+        <v>8.3564725728215014E-4</v>
+      </c>
+      <c r="P125" s="113">
+        <v>1.19694895952429E-4</v>
+      </c>
+      <c r="Q125" s="113">
+        <v>-1.7351101516544632E-4</v>
+      </c>
+    </row>
+    <row r="126" spans="2:18">
+      <c r="N126" s="109">
+        <v>-12.932388411852086</v>
+      </c>
+      <c r="O126" s="109">
+        <v>-14.07591997316697</v>
+      </c>
+      <c r="P126" s="109">
+        <v>-14.287728675789939</v>
+      </c>
+      <c r="Q126" s="109">
+        <v>-14.373003047213039</v>
+      </c>
+    </row>
+    <row r="127" spans="2:18">
+      <c r="N127" s="113">
+        <v>-4.2588140385269817</v>
+      </c>
+      <c r="O127" s="113">
+        <v>-2.7296928943881031</v>
+      </c>
+      <c r="P127" s="113">
+        <v>-2.3095500010056003</v>
+      </c>
+      <c r="Q127" s="113">
+        <v>-2.125369663795837</v>
+      </c>
+    </row>
+    <row r="128" spans="2:18">
+      <c r="N128" s="108">
+        <v>-3.203943556271498</v>
+      </c>
+      <c r="O128" s="108">
+        <v>-4.6255338204697996</v>
+      </c>
+      <c r="P128" s="108">
+        <v>-4.8888454768398741</v>
+      </c>
+      <c r="Q128" s="108">
+        <v>-4.9948549830937488</v>
+      </c>
+    </row>
+    <row r="129" spans="14:17">
+      <c r="N129" s="108">
+        <v>596.72919709875691</v>
+      </c>
+      <c r="O129" s="108">
+        <v>628.89045146175556</v>
+      </c>
+      <c r="P129" s="108">
+        <v>635.02329608188086</v>
+      </c>
+      <c r="Q129" s="108">
+        <v>637.49840440172159</v>
+      </c>
+    </row>
+    <row r="130" spans="14:17">
+      <c r="N130" s="108">
+        <v>27.071008377471777</v>
+      </c>
+      <c r="O130" s="108">
+        <v>14.323101342934034</v>
+      </c>
+      <c r="P130" s="108">
+        <v>12.497102909210016</v>
+      </c>
+      <c r="Q130" s="108">
+        <v>11.794028047617013</v>
+      </c>
+    </row>
+    <row r="131" spans="14:17">
+      <c r="N131" s="138">
+        <v>1.3096071787847329E-3</v>
+      </c>
+      <c r="O131" s="138">
+        <v>1.3090187664806957E-3</v>
+      </c>
+      <c r="P131" s="138">
+        <v>1.3194144670629461E-3</v>
+      </c>
+      <c r="Q131" s="138">
+        <v>1.3243524734098794E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="14:17">
+      <c r="N132" s="138">
+        <v>0.30762458130894782</v>
+      </c>
+      <c r="O132" s="138">
+        <v>0.25677546166687626</v>
+      </c>
+      <c r="P132" s="138">
+        <v>0.24512322336126074</v>
+      </c>
+      <c r="Q132" s="138">
+        <v>0.24033164861361092</v>
+      </c>
+    </row>
+    <row r="133" spans="14:17">
+      <c r="N133" s="138">
+        <v>4.8779344027428806</v>
+      </c>
+      <c r="O133" s="138">
+        <v>1.9243426574143996</v>
+      </c>
+      <c r="P133" s="138">
+        <v>1.3004025235480583</v>
+      </c>
+      <c r="Q133" s="138">
+        <v>1.0454948273519165</v>
+      </c>
+    </row>
+    <row r="134" spans="14:17">
+      <c r="N134" s="112"/>
+      <c r="O134" s="112"/>
+      <c r="P134" s="112"/>
+      <c r="Q134" s="112"/>
+    </row>
+    <row r="135" spans="14:17">
+      <c r="N135" s="109">
+        <v>1.6561002853128552</v>
+      </c>
+      <c r="O135" s="109">
+        <v>1.0308793776934759</v>
+      </c>
+      <c r="P135" s="109">
+        <v>0.95151330024544911</v>
+      </c>
+      <c r="Q135" s="109">
+        <v>0.92207300837622941</v>
       </c>
     </row>
   </sheetData>
@@ -42323,6 +42525,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -42575,24 +42794,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42609,29 +42836,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>